<commit_message>
Update old units of paint from g to PT Add tapping operation to Prewetter Correct threaded stud to have proper length in M258A
</commit_message>
<xml_diff>
--- a/OpsAndMats/M258A.xlsx
+++ b/OpsAndMats/M258A.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eclark.LABTESTING\Documents\ERP Notes\Phase2_BOM\OpsAndMats\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3575B2-35CD-4DEC-B4E8-25C85C1599B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Materials" sheetId="1" r:id="rId1"/>
     <sheet name="Operations" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -779,8 +785,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -843,6 +849,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -889,7 +903,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -921,9 +935,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -955,6 +987,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1130,14 +1180,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S21" sqref="S21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:43">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1268,7 +1320,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:43">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -1351,7 +1403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:43">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -1434,7 +1486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:43">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -1469,7 +1521,7 @@
         <v>8</v>
       </c>
       <c r="S4">
-        <v>1.188</v>
+        <v>1.1879999999999999</v>
       </c>
       <c r="T4" t="s">
         <v>199</v>
@@ -1517,7 +1569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:43">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1600,7 +1652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:43">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -1683,7 +1735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:43">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -1766,7 +1818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:43">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -1849,7 +1901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:43">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -1932,7 +1984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:43">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -2015,7 +2067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:43">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -2098,7 +2150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:43">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -2181,7 +2233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:43">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -2264,7 +2316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:43">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -2347,7 +2399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:43">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -2430,7 +2482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:43">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -2513,7 +2565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:43">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -2596,7 +2648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:43">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -2679,7 +2731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:43">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -2762,7 +2814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:43">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -2797,13 +2849,13 @@
         <v>8</v>
       </c>
       <c r="S20">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="T20" t="s">
         <v>199</v>
       </c>
       <c r="U20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="V20">
         <v>0</v>
@@ -2845,7 +2897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:43">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>55</v>
       </c>
@@ -2928,7 +2980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:43">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>56</v>
       </c>
@@ -3011,7 +3063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:43">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -3094,7 +3146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:43">
+    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -3177,7 +3229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:43">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>58</v>
       </c>
@@ -3260,7 +3312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:43">
+    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>58</v>
       </c>
@@ -3343,7 +3395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:43">
+    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>58</v>
       </c>
@@ -3426,7 +3478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:43">
+    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>59</v>
       </c>
@@ -3509,7 +3561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:43">
+    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>60</v>
       </c>
@@ -3592,7 +3644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:43">
+    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>60</v>
       </c>
@@ -3675,7 +3727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:43">
+    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>60</v>
       </c>
@@ -3758,7 +3810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:43">
+    <row r="32" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -3841,7 +3893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:43">
+    <row r="33" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>62</v>
       </c>
@@ -3924,7 +3976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:43">
+    <row r="34" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>63</v>
       </c>
@@ -4007,7 +4059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:43">
+    <row r="35" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>64</v>
       </c>
@@ -4090,7 +4142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:43">
+    <row r="36" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>65</v>
       </c>
@@ -4173,7 +4225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:43">
+    <row r="37" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>66</v>
       </c>
@@ -4256,7 +4308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:43">
+    <row r="38" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>67</v>
       </c>
@@ -4339,7 +4391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:43">
+    <row r="39" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>67</v>
       </c>
@@ -4422,7 +4474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:43">
+    <row r="40" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>67</v>
       </c>
@@ -4505,7 +4557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:43">
+    <row r="41" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>67</v>
       </c>
@@ -4588,7 +4640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:43">
+    <row r="42" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>67</v>
       </c>
@@ -4671,7 +4723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:43">
+    <row r="43" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>67</v>
       </c>
@@ -4754,7 +4806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:43">
+    <row r="44" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>67</v>
       </c>
@@ -4837,7 +4889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:43">
+    <row r="45" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>67</v>
       </c>
@@ -4920,7 +4972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:43">
+    <row r="46" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>67</v>
       </c>
@@ -5003,7 +5055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:43">
+    <row r="47" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>67</v>
       </c>
@@ -5086,7 +5138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:43">
+    <row r="48" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>67</v>
       </c>
@@ -5169,7 +5221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:43">
+    <row r="49" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>67</v>
       </c>
@@ -5252,7 +5304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:43">
+    <row r="50" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>67</v>
       </c>
@@ -5335,7 +5387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:43">
+    <row r="51" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>67</v>
       </c>
@@ -5418,7 +5470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:43">
+    <row r="52" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>67</v>
       </c>
@@ -5501,7 +5553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:43">
+    <row r="53" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>67</v>
       </c>
@@ -5584,7 +5636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:43">
+    <row r="54" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>67</v>
       </c>
@@ -5667,7 +5719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:43">
+    <row r="55" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>67</v>
       </c>
@@ -5750,7 +5802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:43">
+    <row r="56" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>67</v>
       </c>
@@ -5833,7 +5885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:43">
+    <row r="57" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>67</v>
       </c>
@@ -5916,7 +5968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:43">
+    <row r="58" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>67</v>
       </c>
@@ -5999,7 +6051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:43">
+    <row r="59" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>67</v>
       </c>
@@ -6082,7 +6134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:43">
+    <row r="60" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>67</v>
       </c>
@@ -6165,7 +6217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:43">
+    <row r="61" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>67</v>
       </c>
@@ -6248,7 +6300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:43">
+    <row r="62" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>67</v>
       </c>
@@ -6331,7 +6383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:43">
+    <row r="63" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>67</v>
       </c>
@@ -6414,7 +6466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:43">
+    <row r="64" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>67</v>
       </c>
@@ -6497,7 +6549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:43">
+    <row r="65" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>67</v>
       </c>
@@ -6580,7 +6632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:43">
+    <row r="66" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>67</v>
       </c>
@@ -6663,7 +6715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:43">
+    <row r="67" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -6746,7 +6798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:43">
+    <row r="68" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -6829,7 +6881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:43">
+    <row r="69" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -6912,7 +6964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:43">
+    <row r="70" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>67</v>
       </c>
@@ -6995,7 +7047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:43">
+    <row r="71" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>67</v>
       </c>
@@ -7078,7 +7130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:43">
+    <row r="72" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>67</v>
       </c>
@@ -7161,7 +7213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:43">
+    <row r="73" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>67</v>
       </c>
@@ -7244,7 +7296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:43">
+    <row r="74" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>67</v>
       </c>
@@ -7327,7 +7379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:43">
+    <row r="75" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>67</v>
       </c>
@@ -7410,7 +7462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:43">
+    <row r="76" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>67</v>
       </c>
@@ -7493,7 +7545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:43">
+    <row r="77" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>67</v>
       </c>
@@ -7576,7 +7628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:43">
+    <row r="78" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>67</v>
       </c>
@@ -7659,7 +7711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:43">
+    <row r="79" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>67</v>
       </c>
@@ -7742,7 +7794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:43">
+    <row r="80" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>67</v>
       </c>
@@ -7825,7 +7877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:43">
+    <row r="81" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>67</v>
       </c>
@@ -7908,7 +7960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:43">
+    <row r="82" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>67</v>
       </c>
@@ -7991,7 +8043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:43">
+    <row r="83" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>68</v>
       </c>
@@ -8074,7 +8126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:43">
+    <row r="84" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>68</v>
       </c>
@@ -8157,7 +8209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:43">
+    <row r="85" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>69</v>
       </c>
@@ -8240,7 +8292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:43">
+    <row r="86" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>69</v>
       </c>
@@ -8329,14 +8381,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AW75"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:49">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8485,7 +8537,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="2" spans="1:49">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -8595,7 +8647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:49">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -8705,7 +8757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:49">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -8815,7 +8867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:49">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -8925,7 +8977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:49">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -9035,7 +9087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:49">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -9145,7 +9197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:49">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -9255,7 +9307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:49">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -9365,7 +9417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:49">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -9475,7 +9527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:49">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -9585,7 +9637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:49">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -9695,7 +9747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:49">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -9805,7 +9857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:49">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -9915,7 +9967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:49">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -10025,7 +10077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:49">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -10135,7 +10187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:49">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -10245,7 +10297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:49">
+    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -10355,7 +10407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:49">
+    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -10465,7 +10517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:49">
+    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -10575,7 +10627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:49">
+    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -10685,7 +10737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:49">
+    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>49</v>
       </c>
@@ -10795,7 +10847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:49">
+    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>50</v>
       </c>
@@ -10905,7 +10957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:49">
+    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -11015,7 +11067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:49">
+    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -11125,7 +11177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:49">
+    <row r="26" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>51</v>
       </c>
@@ -11235,7 +11287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:49">
+    <row r="27" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -11345,7 +11397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:49">
+    <row r="28" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -11455,7 +11507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:49">
+    <row r="29" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>52</v>
       </c>
@@ -11565,7 +11617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:49">
+    <row r="30" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -11675,7 +11727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:49">
+    <row r="31" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -11785,7 +11837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:49">
+    <row r="32" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -11895,7 +11947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:49">
+    <row r="33" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>53</v>
       </c>
@@ -12005,7 +12057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:49">
+    <row r="34" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>53</v>
       </c>
@@ -12115,7 +12167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:49">
+    <row r="35" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>53</v>
       </c>
@@ -12225,7 +12277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:49">
+    <row r="36" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>54</v>
       </c>
@@ -12335,7 +12387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:49">
+    <row r="37" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>54</v>
       </c>
@@ -12445,7 +12497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:49">
+    <row r="38" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>55</v>
       </c>
@@ -12555,7 +12607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:49">
+    <row r="39" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>55</v>
       </c>
@@ -12665,7 +12717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:49">
+    <row r="40" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>56</v>
       </c>
@@ -12775,7 +12827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:49">
+    <row r="41" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>56</v>
       </c>
@@ -12885,7 +12937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:49">
+    <row r="42" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>56</v>
       </c>
@@ -12995,7 +13047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:49">
+    <row r="43" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>56</v>
       </c>
@@ -13105,7 +13157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:49">
+    <row r="44" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>57</v>
       </c>
@@ -13215,7 +13267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:49">
+    <row r="45" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>57</v>
       </c>
@@ -13325,7 +13377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:49">
+    <row r="46" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>57</v>
       </c>
@@ -13435,7 +13487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:49">
+    <row r="47" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>57</v>
       </c>
@@ -13545,7 +13597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:49">
+    <row r="48" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>58</v>
       </c>
@@ -13655,7 +13707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:49">
+    <row r="49" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>58</v>
       </c>
@@ -13765,7 +13817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:49">
+    <row r="50" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -13875,7 +13927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:49">
+    <row r="51" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>59</v>
       </c>
@@ -13985,7 +14037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:49">
+    <row r="52" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>59</v>
       </c>
@@ -14095,7 +14147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:49">
+    <row r="53" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>59</v>
       </c>
@@ -14205,7 +14257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:49">
+    <row r="54" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>59</v>
       </c>
@@ -14315,7 +14367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:49">
+    <row r="55" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -14425,7 +14477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:49">
+    <row r="56" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>61</v>
       </c>
@@ -14535,7 +14587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:49">
+    <row r="57" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>61</v>
       </c>
@@ -14645,7 +14697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:49">
+    <row r="58" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>61</v>
       </c>
@@ -14755,7 +14807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:49">
+    <row r="59" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>62</v>
       </c>
@@ -14865,7 +14917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:49">
+    <row r="60" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>62</v>
       </c>
@@ -14975,7 +15027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:49">
+    <row r="61" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>62</v>
       </c>
@@ -15085,7 +15137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:49">
+    <row r="62" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>63</v>
       </c>
@@ -15195,7 +15247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:49">
+    <row r="63" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -15305,7 +15357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:49">
+    <row r="64" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -15415,7 +15467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:49">
+    <row r="65" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -15525,7 +15577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:49">
+    <row r="66" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -15635,7 +15687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:49">
+    <row r="67" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -15745,7 +15797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:49">
+    <row r="68" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>65</v>
       </c>
@@ -15855,7 +15907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:49">
+    <row r="69" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>66</v>
       </c>
@@ -15965,7 +16017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:49">
+    <row r="70" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>66</v>
       </c>
@@ -16075,7 +16127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:49">
+    <row r="71" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>66</v>
       </c>
@@ -16185,7 +16237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:49">
+    <row r="72" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>66</v>
       </c>
@@ -16295,7 +16347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:49">
+    <row r="73" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>67</v>
       </c>
@@ -16405,7 +16457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:49">
+    <row r="74" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>68</v>
       </c>
@@ -16515,7 +16567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:49">
+    <row r="75" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>69</v>
       </c>

</xml_diff>